<commit_message>
Added Data for 2122
</commit_message>
<xml_diff>
--- a/41/Evaluation/Data/Datasheet.xlsx
+++ b/41/Evaluation/Data/Datasheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Moritz/Documents/GitHub/C-Praktikum/41/Evaluation/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E09A3EC-F755-AA4B-869E-392D9E3EF0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ED046F-3FB2-1D44-A851-52B177474465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="2040" windowWidth="28040" windowHeight="17440" xr2:uid="{5636997B-C694-9C41-AC0B-D56DC7215F95}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="2122" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,14 +35,57 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+  <si>
+    <t>Frequency [Hz]</t>
+  </si>
+  <si>
+    <t>Voltage (U_PP) [V]</t>
+  </si>
+  <si>
+    <t>div [V]</t>
+  </si>
+  <si>
+    <t>Wavelength ratio</t>
+  </si>
+  <si>
+    <t>λ/4</t>
+  </si>
+  <si>
+    <t>3λ/4</t>
+  </si>
+  <si>
+    <t>λ/2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -66,8 +109,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +459,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27A1AC3-8CCF-2F4A-A771-0E06F5ECE0A3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>939991</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>933991</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.37E-2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>944991</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>935991</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>937991</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2877970</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2.64E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2874970</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2877970</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2867970</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2.64E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2871970</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1914980</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1889980</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1891980</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2.18E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1890980</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2.18E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1894980</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2.18E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>